<commit_message>
speaking story completed for lesson1
</commit_message>
<xml_diff>
--- a/public/docs/Speaking_stories.xlsx
+++ b/public/docs/Speaking_stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD9162B-C11C-40C9-A09C-6E200B921387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AAB736-B701-4BB2-947A-EAC8B7CD81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B3869C71-3D6A-4C15-B9E8-2F98229CC412}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="42">
   <si>
     <t>\n \n</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>//LESSON 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Hello, my name is Lena. \n I am from Ukraine.\n I arrived in the UK in February 2023. \n I live in Stratford-upon-Avon. \n I work in Coffee #1 in the the center of the town \n I am learning English now. \n  I like meeting new people. \n In my free time, I enjoy reading, walking along the canal. \n I am happy to be here!'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Привіт, мене звати Лєна. \n Я з України. \n Я нещодавно приїхала до Великої Британії. \n Живу в Стратфорді. \n Я працюю в кавярні Coffee #1. \n Зараз я вивчаю англійську мову. \n Мені подобається знайомитися з новими людьми. \n У вільний час я люблю читати і гуляти вздовж каналу. \n Я рада бути тут!',</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -212,6 +218,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6079E66B-7A53-4D81-B55B-9E9D03BABF8C}">
-  <dimension ref="A1:B213"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B208" sqref="B208"/>
+      <selection pane="bottomLeft" activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1362,162 +1374,164 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B161" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B162" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B163" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B164" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B165" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B166" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B167" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B168" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B169" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B170" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B171" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B172" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B173" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B174" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B175" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="176" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="C175" s="5"/>
+    </row>
+    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B176" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B177" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="C177" s="4"/>
+    </row>
+    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B178" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B179" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B180" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B181" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B182" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B183" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B184" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B185" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B186" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B187" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B188" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B189" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B190" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B191" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B192" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>